<commit_message>
Creation of one methods one to calculate the serializable work the parallelizable work
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martim Figueiredo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDC39B9-FC67-4E32-B38E-CE1CF8D75B69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8427AD4C-3504-4BE8-8971-94F7F37C8DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25500" yWindow="3570" windowWidth="9600" windowHeight="4905" xr2:uid="{93F458CE-F793-4DD3-866D-275AA322B0B2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93F458CE-F793-4DD3-866D-275AA322B0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="test-1" sheetId="2" r:id="rId1"/>
     <sheet name="Folha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">'test-1'!$A$1:$J$73</definedName>
+    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">'test-1'!$A$1:$J$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="54">
   <si>
     <t>Column1</t>
   </si>
@@ -197,6 +197,18 @@
   <si>
     <t>Percentagem Trabalho Paralelizavel</t>
   </si>
+  <si>
+    <t>serial Work</t>
+  </si>
+  <si>
+    <t>1-f</t>
+  </si>
+  <si>
+    <t>Column40</t>
+  </si>
+  <si>
+    <t>Column41</t>
+  </si>
 </sst>
 </file>
 
@@ -262,7 +274,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
@@ -345,31 +363,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>SpeedUp por teste</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -404,7 +397,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -421,37 +414,37 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'test-1'!$N$33:$N$39</c:f>
+              <c:f>'test-1'!$O$61:$O$67</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.33200319233838782</c:v>
+                  <c:v>0.66799680766161218</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.87795275590551192</c:v>
+                  <c:v>0.12204724409448808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3846586119696542</c:v>
+                  <c:v>0.38465861196965423</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4919484883258707</c:v>
+                <c:pt idx="3" formatCode="0.000000">
+                  <c:v>0.49194848832587068</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5793559271539253</c:v>
+                  <c:v>0.57935592715392525</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5161363419403318</c:v>
+                  <c:v>0.51613634194033176</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4647885084730654</c:v>
+                  <c:v>0.46478850847306541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C6D8-4CBA-9BEC-8C71D366A1CA}"/>
+              <c16:uniqueId val="{00000000-F35A-4F1B-BAB6-E120278C590F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -470,184 +463,37 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'test-1'!$O$33:$O$39</c:f>
+              <c:f>'test-1'!$P$61:$P$67</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.15536881419234358</c:v>
+                  <c:v>0.33200319233838782</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7513477088948789</c:v>
+                  <c:v>0.87795275590551192</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5778014941302025</c:v>
+                  <c:v>0.61534138803034577</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.6777483827254553</c:v>
+                <c:pt idx="3" formatCode="0.000000">
+                  <c:v>0.50805151167412932</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0906164723040375</c:v>
+                  <c:v>0.42064407284607475</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.929899790902855</c:v>
+                  <c:v>0.48386365805966824</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9736836099511033</c:v>
+                  <c:v>0.53521149152693459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C6D8-4CBA-9BEC-8C71D366A1CA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'test-1'!$P$33:$P$39</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>9.6894409937888198E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.35206820334701616</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.78965922444183312</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.82034278550337336</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1593014941656039</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1281806991895802</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1249463309977803</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C6D8-4CBA-9BEC-8C71D366A1CA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'test-1'!$Q$33:$Q$39</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>7.7079859181026472E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.28277064511016009</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.64604090194022001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.80172177529865052</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1841522731037391</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1466341411324468</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1411125268524147</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-C6D8-4CBA-9BEC-8C71D366A1CA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'test-1'!$R$33:$R$39</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>5.9896160790475742E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.2105679858172154E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.12910888322213293</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.30860558431516621</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0823846157022574</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1379012090003768</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1264041893204497</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-C6D8-4CBA-9BEC-8C71D366A1CA}"/>
+              <c16:uniqueId val="{00000001-F35A-4F1B-BAB6-E120278C590F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -659,19 +505,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="581272464"/>
-        <c:axId val="581272792"/>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="479145512"/>
+        <c:axId val="479143544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="581272464"/>
+        <c:axId val="479145512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -708,7 +553,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="581272792"/>
+        <c:crossAx val="479143544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -716,7 +561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="581272792"/>
+        <c:axId val="479143544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,7 +581,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -767,7 +612,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="581272464"/>
+        <c:crossAx val="479145512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -895,7 +740,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1099,22 +944,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1219,8 +1065,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1352,19 +1198,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1401,23 +1248,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>944217</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>43346</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>509587</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>94698</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="34" name="Gráfico 33">
+        <xdr:cNvPr id="8" name="Gráfico 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CCAD507-3DCB-4F8C-801E-04BE7F68527B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9CBC978-D8BA-463B-86C6-A78C0D8EE0A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1440,8 +1287,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_1" connectionId="1" xr16:uid="{0F42F066-3D54-4ECE-A07C-8F6B24D09921}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="40" unboundColumnsRight="8">
-    <queryTableFields count="18">
+  <queryTableRefresh nextId="42" unboundColumnsRight="10">
+    <queryTableFields count="20">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="6" name="Column6" tableColumnId="6"/>
@@ -1460,6 +1307,8 @@
       <queryTableField id="37" dataBound="0" tableColumnId="37"/>
       <queryTableField id="38" dataBound="0" tableColumnId="38"/>
       <queryTableField id="39" dataBound="0" tableColumnId="39"/>
+      <queryTableField id="40" dataBound="0" tableColumnId="3"/>
+      <queryTableField id="41" dataBound="0" tableColumnId="4"/>
     </queryTableFields>
     <queryTableDeletedFields count="21">
       <deletedField name="Column29"/>
@@ -1489,27 +1338,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F31DADF-08F0-4056-ACE1-11F0C77EA9B6}" name="test_1" displayName="test_1" ref="A1:R73" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:R73" xr:uid="{3A604104-C2EC-4218-89B0-5278CC679D80}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{87114CC1-E8ED-402F-9EB1-EF80973CFC1D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{17F62378-4150-4800-8176-0B791ADF3BA7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{822526B0-BDFE-42EA-98A9-71DF100DB53F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{DF67EE12-857A-43DA-8012-AE33E31F468C}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{ADC3F616-9533-4B3D-A667-FB082B4ED7A8}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{16F73375-BA09-48CB-8925-1168C51C62C9}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="12"/>
-    <tableColumn id="22" xr3:uid="{A90A1F88-8574-44AA-A299-8F0A3C25FA3D}" uniqueName="22" name="Column22" queryTableFieldId="22" dataDxfId="11"/>
-    <tableColumn id="26" xr3:uid="{556FAF2C-1BB7-4DB1-A076-BF4F0AF7A0FC}" uniqueName="26" name="Column26" queryTableFieldId="26" dataDxfId="10"/>
-    <tableColumn id="30" xr3:uid="{B93CE766-FBCC-4B3D-978D-28E621225A61}" uniqueName="30" name="Column30" queryTableFieldId="30" dataDxfId="9"/>
-    <tableColumn id="31" xr3:uid="{1ACE7AA0-4477-44C1-A74E-15D06FD674C6}" uniqueName="31" name="Column31" queryTableFieldId="31" dataDxfId="8"/>
-    <tableColumn id="32" xr3:uid="{5E198B09-023C-4F74-9E2C-DAECC8AFF71C}" uniqueName="32" name="Column32" queryTableFieldId="32" dataDxfId="7"/>
-    <tableColumn id="33" xr3:uid="{59069F89-4DEE-4EAC-AF31-FB443A2EDE7B}" uniqueName="33" name="Column33" queryTableFieldId="33" dataDxfId="6"/>
-    <tableColumn id="34" xr3:uid="{2CC94392-1A91-4923-8660-1F10F8330A1D}" uniqueName="34" name="Column34" queryTableFieldId="34" dataDxfId="5"/>
-    <tableColumn id="35" xr3:uid="{D3E1DDF8-0E49-436C-BAF4-756FD49A80A1}" uniqueName="35" name="Column35" queryTableFieldId="35" dataDxfId="4"/>
-    <tableColumn id="36" xr3:uid="{2906BC31-D285-493F-9A63-8716325B8D09}" uniqueName="36" name="Column36" queryTableFieldId="36" dataDxfId="3"/>
-    <tableColumn id="37" xr3:uid="{469EEEE7-E5FC-47A5-A86A-A0BA5308AC9E}" uniqueName="37" name="Column37" queryTableFieldId="37" dataDxfId="2"/>
-    <tableColumn id="38" xr3:uid="{0E6A9588-3391-45F8-9303-BEDC2E5D37EC}" uniqueName="38" name="Column38" queryTableFieldId="38" dataDxfId="1"/>
-    <tableColumn id="39" xr3:uid="{67232F97-B4E6-4541-9FF2-2DC3E6873E45}" uniqueName="39" name="Column39" queryTableFieldId="39" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F31DADF-08F0-4056-ACE1-11F0C77EA9B6}" name="test_1" displayName="test_1" ref="A1:T76" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:T76" xr:uid="{3A604104-C2EC-4218-89B0-5278CC679D80}"/>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{87114CC1-E8ED-402F-9EB1-EF80973CFC1D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{17F62378-4150-4800-8176-0B791ADF3BA7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{822526B0-BDFE-42EA-98A9-71DF100DB53F}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{DF67EE12-857A-43DA-8012-AE33E31F468C}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{ADC3F616-9533-4B3D-A667-FB082B4ED7A8}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{16F73375-BA09-48CB-8925-1168C51C62C9}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="14"/>
+    <tableColumn id="22" xr3:uid="{A90A1F88-8574-44AA-A299-8F0A3C25FA3D}" uniqueName="22" name="Column22" queryTableFieldId="22" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{556FAF2C-1BB7-4DB1-A076-BF4F0AF7A0FC}" uniqueName="26" name="Column26" queryTableFieldId="26" dataDxfId="12"/>
+    <tableColumn id="30" xr3:uid="{B93CE766-FBCC-4B3D-978D-28E621225A61}" uniqueName="30" name="Column30" queryTableFieldId="30" dataDxfId="11"/>
+    <tableColumn id="31" xr3:uid="{1ACE7AA0-4477-44C1-A74E-15D06FD674C6}" uniqueName="31" name="Column31" queryTableFieldId="31" dataDxfId="10"/>
+    <tableColumn id="32" xr3:uid="{5E198B09-023C-4F74-9E2C-DAECC8AFF71C}" uniqueName="32" name="Column32" queryTableFieldId="32" dataDxfId="9"/>
+    <tableColumn id="33" xr3:uid="{59069F89-4DEE-4EAC-AF31-FB443A2EDE7B}" uniqueName="33" name="Column33" queryTableFieldId="33" dataDxfId="8"/>
+    <tableColumn id="34" xr3:uid="{2CC94392-1A91-4923-8660-1F10F8330A1D}" uniqueName="34" name="Column34" queryTableFieldId="34" dataDxfId="7"/>
+    <tableColumn id="35" xr3:uid="{D3E1DDF8-0E49-436C-BAF4-756FD49A80A1}" uniqueName="35" name="Column35" queryTableFieldId="35" dataDxfId="6"/>
+    <tableColumn id="36" xr3:uid="{2906BC31-D285-493F-9A63-8716325B8D09}" uniqueName="36" name="Column36" queryTableFieldId="36" dataDxfId="5"/>
+    <tableColumn id="37" xr3:uid="{469EEEE7-E5FC-47A5-A86A-A0BA5308AC9E}" uniqueName="37" name="Column37" queryTableFieldId="37" dataDxfId="4"/>
+    <tableColumn id="38" xr3:uid="{0E6A9588-3391-45F8-9303-BEDC2E5D37EC}" uniqueName="38" name="Column38" queryTableFieldId="38" dataDxfId="3"/>
+    <tableColumn id="39" xr3:uid="{67232F97-B4E6-4541-9FF2-2DC3E6873E45}" uniqueName="39" name="Column39" queryTableFieldId="39" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{444239A4-D48F-4214-8173-DE237F5B6A02}" uniqueName="3" name="Column40" queryTableFieldId="40" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{18047E53-CFC7-4539-8EE8-3599A2451977}" uniqueName="4" name="Column41" queryTableFieldId="41" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1813,10 +1664,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E4E511-0C23-427F-B6A8-E376B21557C8}">
   <sheetPr codeName="Folha1"/>
-  <dimension ref="A1:U73"/>
+  <dimension ref="A1:AB87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L3" zoomScale="71" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="C48" zoomScale="46" workbookViewId="0">
+      <selection activeCell="O61" sqref="O61:P67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1837,7 +1688,7 @@
     <col min="19" max="31" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1892,8 +1743,14 @@
       <c r="R1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1932,8 +1789,10 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1972,8 +1831,10 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2028,8 +1889,10 @@
       <c r="R4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -2082,8 +1945,10 @@
       <c r="R5" s="2">
         <v>2.6082400000000006E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2136,8 +2001,10 @@
       <c r="R6" s="2">
         <v>1.6207900000000004E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2190,8 +2057,10 @@
       <c r="R7" s="2">
         <v>1.2336E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2244,8 +2113,10 @@
       <c r="R8" s="2">
         <v>4.1893299999999994E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2298,8 +2169,10 @@
       <c r="R9" s="2">
         <v>0.14903940000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2352,8 +2225,10 @@
       <c r="R10" s="2">
         <v>1.3632723999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2406,8 +2281,10 @@
       <c r="R11" s="2">
         <v>6.7343466000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2446,8 +2323,10 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2502,8 +2381,10 @@
       <c r="R13" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2556,8 +2437,10 @@
       <c r="R14" s="2">
         <v>1.2187456594384246E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2610,8 +2493,10 @@
       <c r="R15" s="2">
         <v>1.232628223309851E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -2664,6 +2549,8 @@
       <c r="R16" s="2">
         <v>1.0668169524337339E-2</v>
       </c>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -2718,6 +2605,8 @@
       <c r="R17" s="2">
         <v>1.323953410094177E-2</v>
       </c>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
@@ -2772,6 +2661,8 @@
       <c r="R18" s="2">
         <v>1.4126196106524927E-2</v>
       </c>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -2826,6 +2717,8 @@
       <c r="R19" s="2">
         <v>6.1492609325349029E-2</v>
       </c>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
@@ -2880,6 +2773,8 @@
       <c r="R20" s="2">
         <v>0.1578871780444504</v>
       </c>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -2920,6 +2815,8 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -2976,6 +2873,8 @@
       <c r="R22" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -3030,6 +2929,8 @@
       <c r="R23" s="1">
         <v>2.4804833333333332E-2</v>
       </c>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
@@ -3084,6 +2985,8 @@
       <c r="R24" s="1">
         <v>1.7181571428571428E-2</v>
       </c>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
@@ -3138,6 +3041,8 @@
       <c r="R25" s="1">
         <v>9.5423333333333332E-3</v>
       </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -3192,6 +3097,8 @@
       <c r="R26" s="1">
         <v>4.604119999999999E-2</v>
       </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
@@ -3246,6 +3153,8 @@
       <c r="R27" s="1">
         <v>0.1453014</v>
       </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
@@ -3300,6 +3209,8 @@
       <c r="R28" s="1">
         <v>1.3498681249999998</v>
       </c>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -3354,6 +3265,8 @@
       <c r="R29" s="1">
         <v>6.7344573750000007</v>
       </c>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
       <c r="U29">
         <f>SUM(U53)</f>
         <v>0</v>
@@ -3398,6 +3311,8 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
@@ -3454,6 +3369,8 @@
       <c r="R31" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
@@ -3494,8 +3411,10 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -3544,8 +3463,10 @@
       <c r="R33" s="2">
         <v>5.9896160790475742E-4</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -3594,8 +3515,10 @@
       <c r="R34" s="2">
         <v>7.2105679858172154E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -3644,8 +3567,10 @@
       <c r="R35" s="2">
         <v>0.12910888322213293</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
@@ -3694,8 +3619,10 @@
       <c r="R36" s="2">
         <v>0.30860558431516621</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -3744,8 +3671,10 @@
       <c r="R37" s="2">
         <v>1.0823846157022574</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
@@ -3794,8 +3723,10 @@
       <c r="R38" s="2">
         <v>1.1379012090003768</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -3844,8 +3775,10 @@
       <c r="R39" s="2">
         <v>1.1264041893204497</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -3884,8 +3817,10 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -3926,8 +3861,10 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -3980,8 +3917,10 @@
       <c r="R42" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -4030,8 +3969,10 @@
       <c r="R43" s="2">
         <v>4.9913467325396451E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>10000000</v>
       </c>
@@ -4080,8 +4021,10 @@
       <c r="R44" s="2">
         <v>6.0088066548476794E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -4130,8 +4073,10 @@
       <c r="R45" s="2">
         <v>1.0759073601844411</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -4180,8 +4125,10 @@
       <c r="R46" s="2">
         <v>2.5717132026263854</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -4230,8 +4177,10 @@
       <c r="R47" s="2">
         <v>9.0198717975188121</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
@@ -4280,8 +4229,10 @@
       <c r="R48" s="2">
         <v>9.482510075003141</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -4330,8 +4281,10 @@
       <c r="R49" s="2">
         <v>9.386701577670415</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
@@ -4370,8 +4323,10 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
@@ -4426,8 +4381,10 @@
       <c r="R51" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
@@ -4458,7 +4415,9 @@
       <c r="J52" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K52" s="1"/>
+      <c r="K52" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2">
@@ -4476,8 +4435,10 @@
       <c r="R52" s="2">
         <v>-1820.2430069930072</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
@@ -4509,25 +4470,27 @@
         <v>11</v>
       </c>
       <c r="K53" s="1"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2">
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1">
         <v>-0.27802690582959633</v>
       </c>
-      <c r="O53" s="2">
+      <c r="O53" s="1">
         <v>-0.44125560538116559</v>
       </c>
-      <c r="P53" s="2">
+      <c r="P53" s="1">
         <v>-2.2084304932735423</v>
       </c>
-      <c r="Q53" s="2">
+      <c r="Q53" s="1">
         <v>-2.8987828315182576</v>
       </c>
-      <c r="R53" s="2">
+      <c r="R53" s="1">
         <v>-150.20217809096732</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>100000000</v>
       </c>
@@ -4559,25 +4522,27 @@
         <v>11</v>
       </c>
       <c r="K54" s="1"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2">
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1">
         <v>0.55560064935064912</v>
       </c>
-      <c r="O54" s="2">
+      <c r="O54" s="1">
         <v>0.4882756132756132</v>
       </c>
-      <c r="P54" s="2">
+      <c r="P54" s="1">
         <v>-0.31964285714285717</v>
       </c>
-      <c r="Q54" s="2">
+      <c r="Q54" s="1">
         <v>-0.62615955473098395</v>
       </c>
-      <c r="R54" s="2">
+      <c r="R54" s="1">
         <v>-7.3586186540732008</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
@@ -4609,25 +4574,27 @@
         <v>11</v>
       </c>
       <c r="K55" s="1"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2">
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1">
         <v>0.65947114417856434</v>
       </c>
-      <c r="O55" s="2">
+      <c r="O55" s="1">
         <v>0.53861742297294268</v>
       </c>
-      <c r="P55" s="2">
+      <c r="P55" s="1">
         <v>-0.26280313693947333</v>
       </c>
-      <c r="Q55" s="2">
+      <c r="Q55" s="1">
         <v>-0.28264628996581564</v>
       </c>
-      <c r="R55" s="2">
+      <c r="R55" s="1">
         <v>-2.4440531597901392</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
@@ -4659,25 +4626,27 @@
         <v>11</v>
       </c>
       <c r="K56" s="1"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2">
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1">
         <v>0.7336610034420199</v>
       </c>
-      <c r="O56" s="2">
+      <c r="O56" s="1">
         <v>0.69556291920094759</v>
       </c>
-      <c r="P56" s="2">
+      <c r="P56" s="1">
         <v>0.16489394170608876</v>
       </c>
-      <c r="Q56" s="2">
+      <c r="Q56" s="1">
         <v>0.17773030164301332</v>
       </c>
-      <c r="R56" s="2">
+      <c r="R56" s="1">
         <v>8.3033447553514564E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
@@ -4709,25 +4678,27 @@
         <v>11</v>
       </c>
       <c r="K57" s="1"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2">
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1">
         <v>0.68085742378523451</v>
       </c>
-      <c r="O57" s="2">
+      <c r="O57" s="1">
         <v>0.64245117477857905</v>
       </c>
-      <c r="P57" s="2">
+      <c r="P57" s="1">
         <v>0.13634060495627112</v>
       </c>
-      <c r="Q57" s="2">
+      <c r="Q57" s="1">
         <v>0.14615113013679398</v>
       </c>
-      <c r="R57" s="2">
+      <c r="R57" s="1">
         <v>0.13220627709678076</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
@@ -4759,25 +4730,27 @@
         <v>11</v>
       </c>
       <c r="K58" s="1"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2">
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1">
         <v>0.63461517588989458</v>
       </c>
-      <c r="O58" s="2">
+      <c r="O58" s="1">
         <v>0.65777757221194177</v>
       </c>
-      <c r="P58" s="2">
+      <c r="P58" s="1">
         <v>0.13328244474058581</v>
       </c>
-      <c r="Q58" s="2">
+      <c r="Q58" s="1">
         <v>0.14132826996890951</v>
       </c>
-      <c r="R58" s="2">
+      <c r="R58" s="1">
         <v>0.12242095738463434</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -4809,15 +4782,17 @@
         <v>11</v>
       </c>
       <c r="K59" s="1"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
@@ -4848,16 +4823,34 @@
       <c r="J60" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K60" s="1"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-      <c r="R60" s="2"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="K60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S60" s="2"/>
+      <c r="T60" s="2"/>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -4891,13 +4884,42 @@
       <c r="K61" s="1"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
-      <c r="Q61" s="2"/>
-      <c r="R61" s="2"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="N61" s="1"/>
+      <c r="O61" s="1">
+        <v>0.66799680766161218</v>
+      </c>
+      <c r="P61" s="1">
+        <v>0.33200319233838782</v>
+      </c>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1">
+        <v>0.84463118580765639</v>
+      </c>
+      <c r="S61" s="1">
+        <v>0.15536881419234361</v>
+      </c>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1">
+        <v>0.90310559006211177</v>
+      </c>
+      <c r="V61" s="1">
+        <v>9.6894409937888226E-2</v>
+      </c>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1">
+        <v>0.92292014081897356</v>
+      </c>
+      <c r="Y61">
+        <v>7.7079859181026444E-2</v>
+      </c>
+      <c r="AA61">
+        <v>0.99940103839209526</v>
+      </c>
+      <c r="AB61">
+        <v>5.9896160790473552E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>10</v>
       </c>
@@ -4931,13 +4953,42 @@
       <c r="K62" s="1"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="R62" s="2"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="N62" s="1"/>
+      <c r="O62" s="1">
+        <v>0.12204724409448808</v>
+      </c>
+      <c r="P62" s="1">
+        <v>0.87795275590551192</v>
+      </c>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1">
+        <v>0.2486522911051211</v>
+      </c>
+      <c r="S62" s="1">
+        <v>0.7513477088948789</v>
+      </c>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1">
+        <v>0.64793179665298384</v>
+      </c>
+      <c r="V62" s="1">
+        <v>0.35206820334701616</v>
+      </c>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1">
+        <v>0.71722935488983985</v>
+      </c>
+      <c r="Y62">
+        <v>0.28277064511016015</v>
+      </c>
+      <c r="AA62">
+        <v>0.99278943201418279</v>
+      </c>
+      <c r="AB62">
+        <v>7.2105679858172067E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
@@ -4971,13 +5022,42 @@
       <c r="K63" s="1"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
-      <c r="R63" s="2"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="N63" s="1"/>
+      <c r="O63" s="1">
+        <v>0.38465861196965423</v>
+      </c>
+      <c r="P63" s="1">
+        <v>0.61534138803034577</v>
+      </c>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1">
+        <v>0.57780149413020254</v>
+      </c>
+      <c r="S63" s="1">
+        <v>0.42219850586979746</v>
+      </c>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1">
+        <v>0.21034077555816688</v>
+      </c>
+      <c r="V63" s="1">
+        <v>0.78965922444183312</v>
+      </c>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1">
+        <v>0.35395909805977999</v>
+      </c>
+      <c r="Y63">
+        <v>0.64604090194022001</v>
+      </c>
+      <c r="AA63">
+        <v>0.87089111677786701</v>
+      </c>
+      <c r="AB63">
+        <v>0.12910888322213299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>500000000</v>
       </c>
@@ -5012,12 +5092,41 @@
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
+      <c r="O64" s="2">
+        <v>0.49194848832587068</v>
+      </c>
+      <c r="P64" s="2">
+        <v>0.50805151167412932</v>
+      </c>
       <c r="Q64" s="2"/>
-      <c r="R64" s="2"/>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R64" s="2">
+        <v>0.67774838272545535</v>
+      </c>
+      <c r="S64" s="2">
+        <v>0.32225161727454465</v>
+      </c>
+      <c r="T64" s="2"/>
+      <c r="U64" s="2">
+        <v>0.17965721449662664</v>
+      </c>
+      <c r="V64" s="2">
+        <v>0.82034278550337336</v>
+      </c>
+      <c r="W64" s="2"/>
+      <c r="X64" s="2">
+        <v>0.19827822470134948</v>
+      </c>
+      <c r="Y64">
+        <v>0.80172177529865052</v>
+      </c>
+      <c r="AA64">
+        <v>0.69139441568483373</v>
+      </c>
+      <c r="AB64">
+        <v>0.30860558431516627</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
@@ -5051,13 +5160,42 @@
       <c r="K65" s="1"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="2"/>
-      <c r="O65" s="2"/>
-      <c r="P65" s="2"/>
-      <c r="Q65" s="2"/>
-      <c r="R65" s="2"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="N65" s="1"/>
+      <c r="O65" s="1">
+        <v>0.57935592715392525</v>
+      </c>
+      <c r="P65" s="1">
+        <v>0.42064407284607475</v>
+      </c>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1">
+        <v>1.0906164723040375</v>
+      </c>
+      <c r="S65" s="1">
+        <v>-9.0616472304037465E-2</v>
+      </c>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1">
+        <v>0.15930149416560391</v>
+      </c>
+      <c r="V65" s="1">
+        <v>0.84069850583439609</v>
+      </c>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1">
+        <v>0.18415227310373905</v>
+      </c>
+      <c r="Y65">
+        <v>0.81584772689626095</v>
+      </c>
+      <c r="AA65">
+        <v>8.2384615702257413E-2</v>
+      </c>
+      <c r="AB65">
+        <v>0.91761538429774259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>10</v>
       </c>
@@ -5091,13 +5229,42 @@
       <c r="K66" s="1"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="2"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="N66" s="1"/>
+      <c r="O66" s="1">
+        <v>0.51613634194033176</v>
+      </c>
+      <c r="P66" s="1">
+        <v>0.48386365805966824</v>
+      </c>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1">
+        <v>0.92989979090285502</v>
+      </c>
+      <c r="S66" s="1">
+        <v>7.0100209097144983E-2</v>
+      </c>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1">
+        <v>0.12818069918958019</v>
+      </c>
+      <c r="V66" s="1">
+        <v>0.87181930081041981</v>
+      </c>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1">
+        <v>0.14663414113244677</v>
+      </c>
+      <c r="Y66">
+        <v>0.85336585886755323</v>
+      </c>
+      <c r="AA66">
+        <v>0.13790120900037683</v>
+      </c>
+      <c r="AB66">
+        <v>0.86209879099962317</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
@@ -5131,13 +5298,42 @@
       <c r="K67" s="1"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="N67" s="1"/>
+      <c r="O67" s="1">
+        <v>0.46478850847306541</v>
+      </c>
+      <c r="P67" s="1">
+        <v>0.53521149152693459</v>
+      </c>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1">
+        <v>0.97368360995110326</v>
+      </c>
+      <c r="S67" s="1">
+        <v>2.6316390048896743E-2</v>
+      </c>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1">
+        <v>0.1249463309977803</v>
+      </c>
+      <c r="V67" s="1">
+        <v>0.8750536690022197</v>
+      </c>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1">
+        <v>0.14111252685241471</v>
+      </c>
+      <c r="Y67">
+        <v>0.85888747314758529</v>
+      </c>
+      <c r="AA67">
+        <v>0.12640418932044972</v>
+      </c>
+      <c r="AB67">
+        <v>0.87359581067955028</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>10</v>
       </c>
@@ -5176,8 +5372,10 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>10</v>
       </c>
@@ -5216,8 +5414,10 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S69" s="2"/>
+      <c r="T69" s="2"/>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
@@ -5256,8 +5456,10 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S70" s="2"/>
+      <c r="T70" s="2"/>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
@@ -5296,8 +5498,10 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
@@ -5336,8 +5540,10 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S72" s="2"/>
+      <c r="T72" s="2"/>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>10</v>
       </c>
@@ -5376,6 +5582,68 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+      <c r="S74" s="2"/>
+      <c r="T74" s="2"/>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="2"/>
+      <c r="S75" s="2"/>
+      <c r="T75" s="2"/>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+      <c r="S76" s="2"/>
+      <c r="T76" s="2"/>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="M79" s="2"/>
+    </row>
+    <row r="81" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="M81" s="2"/>
+    </row>
+    <row r="82" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+    </row>
+    <row r="85" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="M85" s="2"/>
+    </row>
+    <row r="87" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="M87" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>